<commit_message>
cambio de float a double
</commit_message>
<xml_diff>
--- a/src/test/resources/datasetEstimacion.xlsx
+++ b/src/test/resources/datasetEstimacion.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="estimacion" sheetId="1" r:id="rId1"/>
+    <sheet name="caso_de_uso" sheetId="2" r:id="rId2"/>
+    <sheet name="actor" sheetId="3" r:id="rId3"/>
+    <sheet name="factor_estimacion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>idestimacion</t>
   </si>
@@ -26,13 +29,46 @@
   </si>
   <si>
     <t>Prueba</t>
+  </si>
+  <si>
+    <t>numcaso</t>
+  </si>
+  <si>
+    <t>complejidad</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>idplataforma</t>
+  </si>
+  <si>
+    <t>Generar reporte nuevo de cascos</t>
+  </si>
+  <si>
+    <t>Generar reporte antiguo de cascos</t>
+  </si>
+  <si>
+    <t>numactor</t>
+  </si>
+  <si>
+    <t>Emisor</t>
+  </si>
+  <si>
+    <t>idfactor</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>11312 - Reporte de Impresión para Cascos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +76,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -57,15 +110,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,23 +455,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="3" width="40.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -392,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -402,4 +491,402 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="D2" name="Rango1"/>
+    <protectedRange sqref="D3" name="Rango1_1"/>
+  </protectedRanges>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="D2" name="Rango2"/>
+  </protectedRanges>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="C2:C14" name="Rango1_2"/>
+    <protectedRange sqref="C15:C22" name="Rango2"/>
+  </protectedRanges>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Complejidad" prompt="Seleccionar la complejidad del factor técnico del proyecto" sqref="C2:C22">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
carga de datos preliminar
</commit_message>
<xml_diff>
--- a/src/test/resources/datasetEstimacion.xlsx
+++ b/src/test/resources/datasetEstimacion.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="estimacion" sheetId="1" r:id="rId1"/>
     <sheet name="caso_de_uso" sheetId="2" r:id="rId2"/>
     <sheet name="actor" sheetId="3" r:id="rId3"/>
     <sheet name="factor_estimacion" sheetId="4" r:id="rId4"/>
+    <sheet name="cronograma" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>idestimacion</t>
   </si>
@@ -62,13 +63,31 @@
   </si>
   <si>
     <t>11312 - Reporte de Impresión para Cascos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idtarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> incluir</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> porcentaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recursos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> horas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +106,14 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -139,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -151,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -625,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -889,4 +917,167 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
avance con los paneles de tareas de cronograma. preparación para incluir los factores
</commit_message>
<xml_diff>
--- a/src/test/resources/datasetEstimacion.xlsx
+++ b/src/test/resources/datasetEstimacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="estimacion" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Prueba</t>
   </si>
   <si>
-    <t>numcaso</t>
-  </si>
-  <si>
     <t>complejidad</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>Generar reporte antiguo de cascos</t>
   </si>
   <si>
-    <t>numactor</t>
-  </si>
-  <si>
     <t>Emisor</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t xml:space="preserve"> horas</t>
+  </si>
+  <si>
+    <t>idcaso</t>
+  </si>
+  <si>
+    <t>idactor</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -526,33 +526,34 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
@@ -562,24 +563,24 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -598,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,19 +610,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -635,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -668,10 +669,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,22 +939,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1071,6 +1072,9 @@
       </c>
       <c r="C8">
         <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.15</v>
       </c>
       <c r="E8">
         <v>1</v>

</xml_diff>

<commit_message>
pintar los costos de cada proveedor y el rango de horas tomando el parámetro de desviación
</commit_message>
<xml_diff>
--- a/src/test/resources/datasetEstimacion.xlsx
+++ b/src/test/resources/datasetEstimacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="10380" windowHeight="6540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="estimacion" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>idestimacion</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>idactor</t>
+  </si>
+  <si>
+    <t>idfactorestimacion</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -652,267 +655,334 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="C2:C14" name="Rango1_2"/>
-    <protectedRange sqref="C15:C22" name="Rango2"/>
+    <protectedRange sqref="D2:D14" name="Rango1_2"/>
+    <protectedRange sqref="D15:D22" name="Rango2"/>
   </protectedRanges>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Complejidad" prompt="Seleccionar la complejidad del factor técnico del proyecto" sqref="C2:C22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Complejidad" prompt="Seleccionar la complejidad del factor técnico del proyecto" sqref="D2:D22">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -924,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>